<commit_message>
Highest score with bi-LSTM (run no. 20)
</commit_message>
<xml_diff>
--- a/Toxic_data_results.xlsx
+++ b/Toxic_data_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishay\Documents\Data Science\Kaggle\Toxic Comments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishay\Documents\Data Science\Kaggle\Toxic Comments\Github\kaggle_toxic_comment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6FFF28-D224-42B9-BC41-3B6EE7016893}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE61CAF-4247-4E09-9CD2-0672F27E66A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{ADB42BFE-F64D-4F40-85EC-95D9868DC300}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="56">
   <si>
     <t>Tokenizer</t>
   </si>
@@ -66,12 +71,6 @@
     <t>Kaggle Score</t>
   </si>
   <si>
-    <t>val score</t>
-  </si>
-  <si>
-    <t>train score</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -114,9 +113,6 @@
     <t>dropout=0.25, recurrent_dropout=0.25</t>
   </si>
   <si>
-    <t>Epocs</t>
-  </si>
-  <si>
     <t>Batch_size</t>
   </si>
   <si>
@@ -127,9 +123,6 @@
   </si>
   <si>
     <t>return_sequences=True</t>
-  </si>
-  <si>
-    <t>Glove300</t>
   </si>
   <si>
     <r>
@@ -151,6 +144,78 @@
       </rPr>
       <t>Trainable=False</t>
     </r>
+  </si>
+  <si>
+    <t>return_sequences=False</t>
+  </si>
+  <si>
+    <t>Glove300 Trainable=False</t>
+  </si>
+  <si>
+    <t>Added Early Stopping</t>
+  </si>
+  <si>
+    <t>Best Val Epoch</t>
+  </si>
+  <si>
+    <t>Val Score</t>
+  </si>
+  <si>
+    <t>Best Epocs</t>
+  </si>
+  <si>
+    <t>Total Epochs</t>
+  </si>
+  <si>
+    <t>Didn't reach max</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Min Word Length</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>53456+200</t>
+  </si>
+  <si>
+    <t>nltk_wordpunkt</t>
+  </si>
+  <si>
+    <t>LSTM 150 x 2</t>
+  </si>
+  <si>
+    <t>LSTM 150 + Conv 64</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>RMSprop</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>Glove300 Trainable=True</t>
+  </si>
+  <si>
+    <t>Bi(LSTM 150)</t>
+  </si>
+  <si>
+    <t>Adam + 0.001</t>
+  </si>
+  <si>
+    <t>Adam + 0.0016</t>
+  </si>
+  <si>
+    <t>Adam + 0.0005</t>
   </si>
 </sst>
 </file>
@@ -205,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -222,6 +287,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -538,36 +621,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166740F3-21FE-41F5-84CC-C554F91AF039}">
-  <dimension ref="A2:T12"/>
+  <dimension ref="A2:W31"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.25" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.25" customWidth="1"/>
     <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="14.58203125" customWidth="1"/>
-    <col min="14" max="14" width="10.4140625" customWidth="1"/>
-    <col min="15" max="15" width="27.75" customWidth="1"/>
-    <col min="16" max="16" width="9.4140625" customWidth="1"/>
-    <col min="20" max="20" width="32.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.58203125" customWidth="1"/>
+    <col min="13" max="13" width="19.9140625" customWidth="1"/>
+    <col min="14" max="14" width="14.58203125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="42.6640625" customWidth="1"/>
+    <col min="17" max="17" width="27.75" customWidth="1"/>
+    <col min="18" max="18" width="9.4140625" customWidth="1"/>
+    <col min="20" max="21" width="10.25" customWidth="1"/>
+    <col min="23" max="23" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -594,34 +681,43 @@
         <v>6</v>
       </c>
       <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
       <c r="Q2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
-      </c>
       <c r="T2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -635,40 +731,46 @@
         <v>200</v>
       </c>
       <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="O3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3">
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>4</v>
       </c>
-      <c r="S3">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -682,40 +784,46 @@
         <v>200</v>
       </c>
       <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4">
+      <c r="O4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>4</v>
       </c>
-      <c r="S4">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -729,40 +837,46 @@
         <v>200</v>
       </c>
       <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="O5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="2">
         <v>1</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>4</v>
       </c>
-      <c r="S5">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -776,40 +890,46 @@
         <v>200</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="O6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="5">
+        <v>23</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="5">
         <v>4</v>
       </c>
-      <c r="S6" s="5">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V6" s="5">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -823,43 +943,49 @@
         <v>200</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="L7" s="5">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>20</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>512</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R7">
-        <v>5</v>
-      </c>
-      <c r="S7">
-        <v>512</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -873,40 +999,46 @@
         <v>200</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="L8" s="5">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T8">
         <v>4</v>
       </c>
-      <c r="S8">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V8">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -920,43 +1052,49 @@
         <v>200</v>
       </c>
       <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="5">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>25</v>
-      </c>
       <c r="O9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T9">
         <v>4</v>
       </c>
-      <c r="S9">
-        <v>512</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V9">
+        <v>512</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -970,41 +1108,49 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="5">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>25</v>
-      </c>
       <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+      <c r="V10">
+        <v>512</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10">
-        <v>2</v>
-      </c>
-      <c r="S10">
-        <v>512</v>
-      </c>
-      <c r="T10" s="4"/>
-    </row>
-    <row r="11" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -1018,46 +1164,52 @@
         <v>200</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="L11" s="7">
+        <v>2</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="7">
+        <v>23</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>50</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="7">
         <v>4</v>
       </c>
-      <c r="S11" s="7">
-        <v>512</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V11" s="7">
+        <v>512</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1071,44 +1223,869 @@
         <v>200</v>
       </c>
       <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="5">
+        <v>2</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12">
+        <v>4</v>
+      </c>
+      <c r="V12">
+        <v>512</v>
+      </c>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.98019999999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="E13">
+        <v>50369</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="5">
+        <v>2</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>50</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>12</v>
+      </c>
+      <c r="V13">
+        <v>512</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.97840000000000005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>50369</v>
+      </c>
+      <c r="F14" s="2">
+        <v>280</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="5">
+        <v>2</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T14">
+        <v>6</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+      <c r="V14">
+        <v>512</v>
+      </c>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0.98029999999999995</v>
+      </c>
+      <c r="E15">
+        <v>53039</v>
+      </c>
+      <c r="F15" s="2">
+        <v>200</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="10">
+        <v>3</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="V15">
+        <v>512</v>
+      </c>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="4">
+        <v>200</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="10">
+        <v>3</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>50</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>512</v>
+      </c>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0.98050000000000004</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="4">
+        <v>150</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="12">
+        <v>3</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>50</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+      <c r="V17">
+        <v>512</v>
+      </c>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="H12" t="s">
+      <c r="C18">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="12">
+        <v>3</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P18" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>49</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="V18">
+        <v>512</v>
+      </c>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" t="s">
-        <v>32</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12">
+      <c r="C19">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R19" t="s">
+        <v>24</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="V19">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>0.9829</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20">
+        <v>200</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="12">
+        <v>3</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R20" s="13">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="V20">
+        <v>512</v>
+      </c>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21">
+        <v>200</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="12">
+        <v>3</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="R21" s="17">
+        <v>0</v>
+      </c>
+      <c r="T21" s="5">
+        <v>6</v>
+      </c>
+      <c r="V21" s="5">
+        <v>512</v>
+      </c>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.9839</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.97829999999999995</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="7">
+        <v>200</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="15">
+        <v>3</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="N22" s="7">
+        <v>0</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7">
         <v>4</v>
       </c>
-      <c r="S12">
-        <v>512</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="V22" s="7">
+        <v>512</v>
+      </c>
+      <c r="W22" s="8"/>
+    </row>
+    <row r="23" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23">
+        <v>200</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="12">
+        <v>3</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R23" s="17">
+        <v>0</v>
+      </c>
+      <c r="T23" s="5">
+        <v>4</v>
+      </c>
+      <c r="V23" s="5">
+        <v>512</v>
+      </c>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24">
+        <v>200</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="12">
+        <v>3</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="R24" s="17">
+        <v>0</v>
+      </c>
+      <c r="T24" s="5">
+        <v>3</v>
+      </c>
+      <c r="V24" s="5">
+        <v>512</v>
+      </c>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.9839</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="5">
+        <v>200</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="12">
+        <v>3</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="R25" s="17">
+        <v>0</v>
+      </c>
+      <c r="T25" s="5">
+        <v>5</v>
+      </c>
+      <c r="V25" s="5">
+        <v>512</v>
+      </c>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.98009999999999997</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="5">
+        <v>200</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="12">
+        <v>3</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="5">
+        <v>0</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R26" s="17">
+        <v>0</v>
+      </c>
+      <c r="T26" s="5">
+        <v>2</v>
+      </c>
+      <c r="V26" s="10">
+        <v>128</v>
+      </c>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="M31" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>